<commit_message>
preparing final clean set of files for submission
</commit_message>
<xml_diff>
--- a/data_from_lab/sep-ROP_Data_good_authorcontact.xlsx
+++ b/data_from_lab/sep-ROP_Data_good_authorcontact.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arm level Data" sheetId="1" r:id="rId1"/>
@@ -1844,8 +1844,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AE249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G157" sqref="G157"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F154" sqref="F154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25042,11 +25042,11 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AU34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>